<commit_message>
add some constraint and a UI using tkinter
</commit_message>
<xml_diff>
--- a/sheet1_error.xlsx
+++ b/sheet1_error.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -491,11 +491,7 @@
       <c r="D2" t="n">
         <v>123456789</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>haja@gmail.com</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>51/13/2001</t>
@@ -503,69 +499,69 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Duplicate Row Error</t>
+          <t>Invalid Email Error</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>gg</t>
+          <t>Fahim</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dfd</t>
+          <t>Malikakkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkkk</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1233</v>
+        <v>1234567</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>gg@gmail.com</t>
+          <t>Malika#gmail.com</t>
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>40129</v>
+        <v>36639</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Duplicate Row Error</t>
+          <t>Invalid Email Error</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>456</v>
+        <v>123</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hfg</t>
+          <t>El hani</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dfdd</t>
+          <t>Hajar</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12333222</v>
+        <v>12345537</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>dfdd@gmail.com</t>
+          <t>hajar@gmail.com</t>
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>37603</v>
+        <v>37588</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Duplicate Row Error</t>
+          <t>Invalid Telephone Error</t>
         </is>
       </c>
     </row>
@@ -598,71 +594,193 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Invalid Date Error</t>
+          <t>Invalid Telephone Error</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>789</v>
+        <v>21</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hamdaoui</t>
+          <t>Alaoui</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mohmed</t>
+          <t>Fatima</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>123456789</v>
+        <v>65434656</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>mohmed@gmail.com</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>12/38-2004</t>
-        </is>
+          <t>Fatima@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>37303</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Invalid Date Error</t>
+          <t>Invalid Telephone Error</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>123</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>dfd</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1233</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>gg@gmail.com</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>40129</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Invalid Telephone Error</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>456</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>hfg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dfdd</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>12333222</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>dfdd@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>37603</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Invalid Telephone Error</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>456</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>El Alami</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ahmed</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>61234567</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Ahmed@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>244/12/2003</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Invalid Date Error</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>789</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hamdaoui</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Mohmed</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>mohmed@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>12/38-2004</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Invalid Date Error</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>21</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>dari</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>hala</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D11" t="n">
         <v>123456789</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>haja@gmail.com</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
         <is>
           <t>51/13/2001</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Invalid Date Error</t>
         </is>

</xml_diff>